<commit_message>
fc fixed dataset and re-trained with marker protein labels only
</commit_message>
<xml_diff>
--- a/FC_figure_bank/Protein + mRNALossAccDF.xlsx
+++ b/FC_figure_bank/Protein + mRNALossAccDF.xlsx
@@ -465,16 +465,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.167630919638802</v>
+        <v>0.1721657006179585</v>
       </c>
       <c r="C2" t="n">
-        <v>0.1696297228336334</v>
+        <v>0.1717537211047279</v>
       </c>
       <c r="D2" t="n">
-        <v>0.239907192575406</v>
+        <v>0.3848653667595172</v>
       </c>
       <c r="E2" t="n">
-        <v>0.2230483271375465</v>
+        <v>0.3840445269016697</v>
       </c>
     </row>
     <row r="3">
@@ -482,16 +482,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>0.190614567083471</v>
+        <v>0.2245537941070164</v>
       </c>
       <c r="C3" t="n">
-        <v>0.165901318192482</v>
+        <v>0.1782604985766941</v>
       </c>
       <c r="D3" t="n">
-        <v>0.239907192575406</v>
+        <v>0.1536675951717734</v>
       </c>
       <c r="E3" t="n">
-        <v>0.3234200743494424</v>
+        <v>0.1020408163265306</v>
       </c>
     </row>
     <row r="4">
@@ -499,16 +499,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>0.181590806473704</v>
+        <v>0.2108696028590202</v>
       </c>
       <c r="C4" t="n">
-        <v>0.161214143037796</v>
+        <v>0.1720033867491616</v>
       </c>
       <c r="D4" t="n">
-        <v>0.2784222737819025</v>
+        <v>0.1731662024141133</v>
       </c>
       <c r="E4" t="n">
-        <v>0.3736059479553903</v>
+        <v>0.1799628942486085</v>
       </c>
     </row>
     <row r="5">
@@ -516,16 +516,16 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>0.1755200365886969</v>
+        <v>0.2062246220953324</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1582038617796368</v>
+        <v>0.1683899097972446</v>
       </c>
       <c r="D5" t="n">
-        <v>0.3025522041763341</v>
+        <v>0.1754874651810585</v>
       </c>
       <c r="E5" t="n">
-        <v>0.4052044609665427</v>
+        <v>0.2226345083487941</v>
       </c>
     </row>
     <row r="6">
@@ -533,16 +533,16 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>0.1731694134719232</v>
+        <v>0.1970847441869623</v>
       </c>
       <c r="C6" t="n">
-        <v>0.1554150879383087</v>
+        <v>0.1636852125326792</v>
       </c>
       <c r="D6" t="n">
-        <v>0.2895591647331787</v>
+        <v>0.212627669452182</v>
       </c>
       <c r="E6" t="n">
-        <v>0.4405204460966543</v>
+        <v>0.3061224489795918</v>
       </c>
     </row>
     <row r="7">
@@ -550,16 +550,16 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>0.1680909500402563</v>
+        <v>0.1863848233924192</v>
       </c>
       <c r="C7" t="n">
-        <v>0.1536197844478819</v>
+        <v>0.1599001271857156</v>
       </c>
       <c r="D7" t="n">
-        <v>0.3169373549883991</v>
+        <v>0.2242339832869081</v>
       </c>
       <c r="E7" t="n">
-        <v>0.4460966542750929</v>
+        <v>0.3970315398886827</v>
       </c>
     </row>
     <row r="8">
@@ -567,16 +567,16 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>0.1633687729344648</v>
+        <v>0.1826099503566237</v>
       </c>
       <c r="C8" t="n">
-        <v>0.1512970593240526</v>
+        <v>0.1566926605171627</v>
       </c>
       <c r="D8" t="n">
-        <v>0.3373549883990719</v>
+        <v>0.2493036211699164</v>
       </c>
       <c r="E8" t="n">
-        <v>0.483271375464684</v>
+        <v>0.4211502782931354</v>
       </c>
     </row>
     <row r="9">
@@ -584,16 +584,16 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>0.1602825347115012</v>
+        <v>0.1754825417609776</v>
       </c>
       <c r="C9" t="n">
-        <v>0.1495873298909929</v>
+        <v>0.1545028256045448</v>
       </c>
       <c r="D9" t="n">
-        <v>0.365661252900232</v>
+        <v>0.2985143918291551</v>
       </c>
       <c r="E9" t="n">
-        <v>0.5074349442379182</v>
+        <v>0.4564007421150278</v>
       </c>
     </row>
     <row r="10">
@@ -601,16 +601,16 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>0.1589235128725276</v>
+        <v>0.1735661617096733</v>
       </c>
       <c r="C10" t="n">
-        <v>0.1479685737027062</v>
+        <v>0.1521397233009338</v>
       </c>
       <c r="D10" t="n">
-        <v>0.3786542923433875</v>
+        <v>0.3129062209842154</v>
       </c>
       <c r="E10" t="n">
-        <v>0.5148698884758365</v>
+        <v>0.4897959183673469</v>
       </c>
     </row>
     <row r="11">
@@ -618,16 +618,16 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>0.1577869351295864</v>
+        <v>0.1694685154977967</v>
       </c>
       <c r="C11" t="n">
-        <v>0.1472032169500987</v>
+        <v>0.150910754998525</v>
       </c>
       <c r="D11" t="n">
-        <v>0.3786542923433875</v>
+        <v>0.3365831012070566</v>
       </c>
       <c r="E11" t="n">
-        <v>0.5204460966542751</v>
+        <v>0.4990723562152133</v>
       </c>
     </row>
     <row r="12">
@@ -635,16 +635,16 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>0.1571133675820687</v>
+        <v>0.1671202077585108</v>
       </c>
       <c r="C12" t="n">
-        <v>0.1456825600730048</v>
+        <v>0.1494412885771857</v>
       </c>
       <c r="D12" t="n">
-        <v>0.3758700696055685</v>
+        <v>0.3426183844011142</v>
       </c>
       <c r="E12" t="n">
-        <v>0.5185873605947955</v>
+        <v>0.5027829313543599</v>
       </c>
     </row>
     <row r="13">
@@ -652,16 +652,16 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>0.1540326050975744</v>
+        <v>0.166834014303544</v>
       </c>
       <c r="C13" t="n">
-        <v>0.1451349722014533</v>
+        <v>0.1491767217715581</v>
       </c>
       <c r="D13" t="n">
-        <v>0.3805104408352668</v>
+        <v>0.3556174558960074</v>
       </c>
       <c r="E13" t="n">
-        <v>0.5353159851301115</v>
+        <v>0.4916512059369202</v>
       </c>
     </row>
     <row r="14">
@@ -669,16 +669,16 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>0.1553163432023104</v>
+        <v>0.1609274197150679</v>
       </c>
       <c r="C14" t="n">
-        <v>0.1434269530905617</v>
+        <v>0.1479512850443522</v>
       </c>
       <c r="D14" t="n">
-        <v>0.4023201856148492</v>
+        <v>0.3853296193129062</v>
       </c>
       <c r="E14" t="n">
-        <v>0.5464684014869888</v>
+        <v>0.5027829313543599</v>
       </c>
     </row>
     <row r="15">
@@ -686,16 +686,16 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>0.1544739297207664</v>
+        <v>0.1624957735047621</v>
       </c>
       <c r="C15" t="n">
-        <v>0.1438874105612437</v>
+        <v>0.1470249791940053</v>
       </c>
       <c r="D15" t="n">
-        <v>0.4129930394431555</v>
+        <v>0.3857938718662953</v>
       </c>
       <c r="E15" t="n">
-        <v>0.5446096654275093</v>
+        <v>0.5120593692022264</v>
       </c>
     </row>
     <row r="16">
@@ -703,16 +703,16 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>0.1522592012496556</v>
+        <v>0.1577271687633851</v>
       </c>
       <c r="C16" t="n">
-        <v>0.1424072451061673</v>
+        <v>0.1463587168190214</v>
       </c>
       <c r="D16" t="n">
-        <v>0.4120649651972158</v>
+        <v>0.4034354688950789</v>
       </c>
       <c r="E16" t="n">
-        <v>0.5557620817843866</v>
+        <v>0.5139146567717996</v>
       </c>
     </row>
     <row r="17">
@@ -720,16 +720,16 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>0.1483521564480136</v>
+        <v>0.1607610109974356</v>
       </c>
       <c r="C17" t="n">
-        <v>0.1421933290031221</v>
+        <v>0.1455059001843134</v>
       </c>
       <c r="D17" t="n">
-        <v>0.4292343387470998</v>
+        <v>0.3992571959145775</v>
       </c>
       <c r="E17" t="n">
-        <v>0.5464684014869888</v>
+        <v>0.5250463821892394</v>
       </c>
     </row>
     <row r="18">
@@ -737,16 +737,16 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>0.1496625314740574</v>
+        <v>0.1562500070123111</v>
       </c>
       <c r="C18" t="n">
-        <v>0.1415488421916962</v>
+        <v>0.1452369954850939</v>
       </c>
       <c r="D18" t="n">
-        <v>0.4218097447795824</v>
+        <v>0.4155060352831941</v>
       </c>
       <c r="E18" t="n">
-        <v>0.5631970260223048</v>
+        <v>0.5083487940630798</v>
       </c>
     </row>
     <row r="19">
@@ -754,16 +754,16 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>0.1475181697922594</v>
+        <v>0.1544222283889266</v>
       </c>
       <c r="C19" t="n">
-        <v>0.1418448868725035</v>
+        <v>0.1443066696325938</v>
       </c>
       <c r="D19" t="n">
-        <v>0.4464037122969838</v>
+        <v>0.435933147632312</v>
       </c>
       <c r="E19" t="n">
-        <v>0.5669144981412639</v>
+        <v>0.5213358070500927</v>
       </c>
     </row>
     <row r="20">
@@ -771,16 +771,16 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>0.1457419320940971</v>
+        <v>0.1565474679364878</v>
       </c>
       <c r="C20" t="n">
-        <v>0.1408835417694516</v>
+        <v>0.1436303241385354</v>
       </c>
       <c r="D20" t="n">
-        <v>0.4524361948955917</v>
+        <v>0.4368616527390901</v>
       </c>
       <c r="E20" t="n">
-        <v>0.5520446096654275</v>
+        <v>0.5176252319109462</v>
       </c>
     </row>
     <row r="21">
@@ -788,16 +788,16 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>0.1459439957843107</v>
+        <v>0.1547195863197832</v>
       </c>
       <c r="C21" t="n">
-        <v>0.1405902935398949</v>
+        <v>0.1436694049172931</v>
       </c>
       <c r="D21" t="n">
-        <v>0.4357308584686775</v>
+        <v>0.4456824512534819</v>
       </c>
       <c r="E21" t="n">
-        <v>0.5724907063197026</v>
+        <v>0.5102040816326531</v>
       </c>
     </row>
     <row r="22">
@@ -805,16 +805,16 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>0.1456330558832954</v>
+        <v>0.1523311712286052</v>
       </c>
       <c r="C22" t="n">
-        <v>0.1398362807101673</v>
+        <v>0.1433470812108782</v>
       </c>
       <c r="D22" t="n">
-        <v>0.4436194895591647</v>
+        <v>0.4345403899721448</v>
       </c>
       <c r="E22" t="n">
-        <v>0.5743494423791822</v>
+        <v>0.5287569573283859</v>
       </c>
     </row>
     <row r="23">
@@ -822,16 +822,16 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>0.1455793016973664</v>
+        <v>0.1541211513035438</v>
       </c>
       <c r="C23" t="n">
-        <v>0.1399428322911263</v>
+        <v>0.1427386196123229</v>
       </c>
       <c r="D23" t="n">
-        <v>0.4561484918793504</v>
+        <v>0.447075208913649</v>
       </c>
       <c r="E23" t="n">
-        <v>0.5669144981412639</v>
+        <v>0.5213358070500927</v>
       </c>
     </row>
     <row r="24">
@@ -839,16 +839,16 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>0.1451073481756098</v>
+        <v>0.1515967859064832</v>
       </c>
       <c r="C24" t="n">
-        <v>0.1395579212241703</v>
+        <v>0.142478364209334</v>
       </c>
       <c r="D24" t="n">
-        <v>0.4607888631090487</v>
+        <v>0.4428969359331476</v>
       </c>
       <c r="E24" t="n">
-        <v>0.5799256505576208</v>
+        <v>0.5287569573283859</v>
       </c>
     </row>
     <row r="25">
@@ -856,16 +856,16 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>0.1452257460092797</v>
+        <v>0.1523419408237233</v>
       </c>
       <c r="C25" t="n">
-        <v>0.1394142889314228</v>
+        <v>0.1418705234924952</v>
       </c>
       <c r="D25" t="n">
-        <v>0.4640371229698376</v>
+        <v>0.447539461467038</v>
       </c>
       <c r="E25" t="n">
-        <v>0.5799256505576208</v>
+        <v>0.5194805194805194</v>
       </c>
     </row>
     <row r="26">
@@ -873,16 +873,16 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>0.1415518373250961</v>
+        <v>0.1489582351025413</v>
       </c>
       <c r="C26" t="n">
-        <v>0.1396111539668507</v>
+        <v>0.141549128625128</v>
       </c>
       <c r="D26" t="n">
-        <v>0.4705336426914153</v>
+        <v>0.4651810584958218</v>
       </c>
       <c r="E26" t="n">
-        <v>0.5817843866171004</v>
+        <v>0.5250463821892394</v>
       </c>
     </row>
     <row r="27">
@@ -890,16 +890,16 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>0.1445765591719571</v>
+        <v>0.1491576115436414</v>
       </c>
       <c r="C27" t="n">
-        <v>0.1391577546795209</v>
+        <v>0.1417088541719649</v>
       </c>
       <c r="D27" t="n">
-        <v>0.4482598607888631</v>
+        <v>0.4707520891364902</v>
       </c>
       <c r="E27" t="n">
-        <v>0.5855018587360595</v>
+        <v>0.5287569573283859</v>
       </c>
     </row>
     <row r="28">
@@ -907,16 +907,16 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>0.1438847057083074</v>
+        <v>0.1491852994350826</v>
       </c>
       <c r="C28" t="n">
-        <v>0.1390639237231678</v>
+        <v>0.1412998967700534</v>
       </c>
       <c r="D28" t="n">
-        <v>0.459860788863109</v>
+        <v>0.4749303621169916</v>
       </c>
       <c r="E28" t="n">
-        <v>0.5929368029739777</v>
+        <v>0.5194805194805194</v>
       </c>
     </row>
     <row r="29">
@@ -924,16 +924,16 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>0.1439665928483009</v>
+        <v>0.1488784227301093</v>
       </c>
       <c r="C29" t="n">
-        <v>0.1380756903025839</v>
+        <v>0.1409318099419276</v>
       </c>
       <c r="D29" t="n">
-        <v>0.4556844547563805</v>
+        <v>0.4535747446610957</v>
       </c>
       <c r="E29" t="n">
-        <v>0.5892193308550185</v>
+        <v>0.5231910946196661</v>
       </c>
     </row>
     <row r="30">
@@ -941,16 +941,16 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>0.1419004138339968</v>
+        <v>0.1480406325529603</v>
       </c>
       <c r="C30" t="n">
-        <v>0.1382456984784868</v>
+        <v>0.1408369061019686</v>
       </c>
       <c r="D30" t="n">
-        <v>0.4459396751740139</v>
+        <v>0.4758588672237697</v>
       </c>
       <c r="E30" t="n">
-        <v>0.587360594795539</v>
+        <v>0.5194805194805194</v>
       </c>
     </row>
     <row r="31">
@@ -958,16 +958,16 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>0.1436342855586725</v>
+        <v>0.1478381713523584</v>
       </c>
       <c r="C31" t="n">
-        <v>0.1381081425481372</v>
+        <v>0.1406014834841093</v>
       </c>
       <c r="D31" t="n">
-        <v>0.459860788863109</v>
+        <v>0.4712163416898793</v>
       </c>
       <c r="E31" t="n">
-        <v>0.587360594795539</v>
+        <v>0.5231910946196661</v>
       </c>
     </row>
     <row r="32">
@@ -975,16 +975,16 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>0.1416612019871964</v>
+        <v>0.1467844497631578</v>
       </c>
       <c r="C32" t="n">
-        <v>0.1379875656631258</v>
+        <v>0.1408614433474011</v>
       </c>
       <c r="D32" t="n">
-        <v>0.4895591647331787</v>
+        <v>0.4823584029712163</v>
       </c>
       <c r="E32" t="n">
-        <v>0.5947955390334573</v>
+        <v>0.5231910946196661</v>
       </c>
     </row>
     <row r="33">
@@ -992,16 +992,16 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>0.140201317913392</v>
+        <v>0.1476099955684999</v>
       </c>
       <c r="C33" t="n">
-        <v>0.1370287901825375</v>
+        <v>0.1406781284345521</v>
       </c>
       <c r="D33" t="n">
-        <v>0.4733178654292343</v>
+        <v>0.4809656453110492</v>
       </c>
       <c r="E33" t="n">
-        <v>0.5762081784386617</v>
+        <v>0.5250463821892394</v>
       </c>
     </row>
     <row r="34">
@@ -1009,16 +1009,16 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>0.141731977901038</v>
+        <v>0.1439723368076717</v>
       </c>
       <c r="C34" t="n">
-        <v>0.1373512016402351</v>
+        <v>0.1407459038827154</v>
       </c>
       <c r="D34" t="n">
-        <v>0.4723897911832947</v>
+        <v>0.5027855153203342</v>
       </c>
       <c r="E34" t="n">
-        <v>0.5947955390334573</v>
+        <v>0.5250463821892394</v>
       </c>
     </row>
     <row r="35">
@@ -1026,16 +1026,16 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>0.1404498662142193</v>
+        <v>0.1455989865695729</v>
       </c>
       <c r="C35" t="n">
-        <v>0.1369699637095133</v>
+        <v>0.1402878868911001</v>
       </c>
       <c r="D35" t="n">
-        <v>0.491415313225058</v>
+        <v>0.4986072423398329</v>
       </c>
       <c r="E35" t="n">
-        <v>0.5910780669144982</v>
+        <v>0.5231910946196661</v>
       </c>
     </row>
     <row r="36">
@@ -1043,16 +1043,16 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>0.1405604354598943</v>
+        <v>0.1456017980680746</v>
       </c>
       <c r="C36" t="n">
-        <v>0.1368931399451362</v>
+        <v>0.1402433100673887</v>
       </c>
       <c r="D36" t="n">
-        <v>0.4733178654292343</v>
+        <v>0.4879294336118848</v>
       </c>
       <c r="E36" t="n">
-        <v>0.5985130111524164</v>
+        <v>0.5287569573283859</v>
       </c>
     </row>
     <row r="37">
@@ -1060,16 +1060,16 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>0.1419291509424939</v>
+        <v>0.1445804941741859</v>
       </c>
       <c r="C37" t="n">
-        <v>0.1371554699209001</v>
+        <v>0.1399689200851652</v>
       </c>
       <c r="D37" t="n">
-        <v>0.4825986078886311</v>
+        <v>0.4916434540389972</v>
       </c>
       <c r="E37" t="n">
-        <v>0.6022304832713755</v>
+        <v>0.5343228200371057</v>
       </c>
     </row>
     <row r="38">
@@ -1077,16 +1077,16 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>0.1401161985362277</v>
+        <v>0.1443463912343278</v>
       </c>
       <c r="C38" t="n">
-        <v>0.1368687980704837</v>
+        <v>0.1399783798389965</v>
       </c>
       <c r="D38" t="n">
-        <v>0.4770301624129931</v>
+        <v>0.4944289693593314</v>
       </c>
       <c r="E38" t="n">
-        <v>0.6022304832713755</v>
+        <v>0.5287569573283859</v>
       </c>
     </row>
     <row r="39">
@@ -1094,16 +1094,16 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>0.1406298514236422</v>
+        <v>0.1459294242017409</v>
       </c>
       <c r="C39" t="n">
-        <v>0.1369994315836165</v>
+        <v>0.1393950225578414</v>
       </c>
       <c r="D39" t="n">
-        <v>0.4812064965197216</v>
+        <v>0.4902506963788301</v>
       </c>
       <c r="E39" t="n">
-        <v>0.5985130111524164</v>
+        <v>0.5306122448979592</v>
       </c>
     </row>
     <row r="40">
@@ -1111,16 +1111,16 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>0.13985150636119</v>
+        <v>0.1441412543987527</v>
       </c>
       <c r="C40" t="n">
-        <v>0.1362383969955974</v>
+        <v>0.1394419074058533</v>
       </c>
       <c r="D40" t="n">
-        <v>0.4965197215777262</v>
+        <v>0.4953574744661096</v>
       </c>
       <c r="E40" t="n">
-        <v>0.587360594795539</v>
+        <v>0.5231910946196661</v>
       </c>
     </row>
     <row r="41">
@@ -1128,16 +1128,16 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>0.1397851346170201</v>
+        <v>0.1436364067827954</v>
       </c>
       <c r="C41" t="n">
-        <v>0.1365111867586772</v>
+        <v>0.1394409967793359</v>
       </c>
       <c r="D41" t="n">
-        <v>0.4802784222737819</v>
+        <v>0.4925719591457753</v>
       </c>
       <c r="E41" t="n">
-        <v>0.5966542750929368</v>
+        <v>0.5213358070500927</v>
       </c>
     </row>
     <row r="42">
@@ -1145,16 +1145,16 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>0.1390807751347037</v>
+        <v>0.1425159393864519</v>
       </c>
       <c r="C42" t="n">
-        <v>0.135676610800955</v>
+        <v>0.1388968245850669</v>
       </c>
       <c r="D42" t="n">
-        <v>0.4867749419953596</v>
+        <v>0.5023212627669452</v>
       </c>
       <c r="E42" t="n">
-        <v>0.5855018587360595</v>
+        <v>0.5287569573283859</v>
       </c>
     </row>
     <row r="43">
@@ -1162,16 +1162,16 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>0.1380351433420882</v>
+        <v>0.1426314691848615</v>
       </c>
       <c r="C43" t="n">
-        <v>0.1364256590604782</v>
+        <v>0.1389097885953056</v>
       </c>
       <c r="D43" t="n">
-        <v>0.4691415313225058</v>
+        <v>0.4995357474466109</v>
       </c>
       <c r="E43" t="n">
-        <v>0.5910780669144982</v>
+        <v>0.5287569573283859</v>
       </c>
     </row>
     <row r="44">
@@ -1179,16 +1179,16 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>0.1378381745341946</v>
+        <v>0.1426660909372217</v>
       </c>
       <c r="C44" t="n">
-        <v>0.1355996628602346</v>
+        <v>0.1393064699239201</v>
       </c>
       <c r="D44" t="n">
-        <v>0.494199535962877</v>
+        <v>0.5204271123491179</v>
       </c>
       <c r="E44" t="n">
-        <v>0.587360594795539</v>
+        <v>0.5287569573283859</v>
       </c>
     </row>
     <row r="45">
@@ -1196,16 +1196,16 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>0.1391460295109188</v>
+        <v>0.1413640130092116</v>
       </c>
       <c r="C45" t="n">
-        <v>0.1355158529347844</v>
+        <v>0.1391764879226685</v>
       </c>
       <c r="D45" t="n">
-        <v>0.5002320185614849</v>
+        <v>0.5092850510677809</v>
       </c>
       <c r="E45" t="n">
-        <v>0.5929368029739777</v>
+        <v>0.5324675324675324</v>
       </c>
     </row>
     <row r="46">
@@ -1213,16 +1213,16 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>0.137889957822421</v>
+        <v>0.1408242092413061</v>
       </c>
       <c r="C46" t="n">
-        <v>0.1352478812138239</v>
+        <v>0.1395024723476834</v>
       </c>
       <c r="D46" t="n">
-        <v>0.4863109048723898</v>
+        <v>0.5060352831940576</v>
       </c>
       <c r="E46" t="n">
-        <v>0.5929368029739777</v>
+        <v>0.5269016697588126</v>
       </c>
     </row>
     <row r="47">
@@ -1230,16 +1230,16 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>0.1377520896494389</v>
+        <v>0.1435642474714448</v>
       </c>
       <c r="C47" t="n">
-        <v>0.1346698742773798</v>
+        <v>0.1386298967732323</v>
       </c>
       <c r="D47" t="n">
-        <v>0.4863109048723898</v>
+        <v>0.4870009285051068</v>
       </c>
       <c r="E47" t="n">
-        <v>0.5910780669144982</v>
+        <v>0.5361781076066791</v>
       </c>
     </row>
     <row r="48">
@@ -1247,16 +1247,16 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>0.1357665219727685</v>
+        <v>0.1406040423933198</v>
       </c>
       <c r="C48" t="n">
-        <v>0.1350807646910349</v>
+        <v>0.1389096420672205</v>
       </c>
       <c r="D48" t="n">
-        <v>0.505800464037123</v>
+        <v>0.5069637883008357</v>
       </c>
       <c r="E48" t="n">
-        <v>0.5780669144981413</v>
+        <v>0.5324675324675324</v>
       </c>
     </row>
     <row r="49">
@@ -1264,16 +1264,16 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>0.1370049844331601</v>
+        <v>0.141973944271312</v>
       </c>
       <c r="C49" t="n">
-        <v>0.1360817957255575</v>
+        <v>0.1386583223938942</v>
       </c>
       <c r="D49" t="n">
-        <v>0.4932714617169374</v>
+        <v>0.5041782729805014</v>
       </c>
       <c r="E49" t="n">
-        <v>0.5836431226765799</v>
+        <v>0.5287569573283859</v>
       </c>
     </row>
     <row r="50">
@@ -1281,16 +1281,16 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>0.1372333127347862</v>
+        <v>0.1403058642411933</v>
       </c>
       <c r="C50" t="n">
-        <v>0.1351710855960846</v>
+        <v>0.1384453665879038</v>
       </c>
       <c r="D50" t="n">
-        <v>0.4997679814385151</v>
+        <v>0.5134633240482822</v>
       </c>
       <c r="E50" t="n">
-        <v>0.5910780669144982</v>
+        <v>0.5306122448979592</v>
       </c>
     </row>
     <row r="51">
@@ -1298,16 +1298,16 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
-        <v>0.1348746857222389</v>
+        <v>0.1415440516875071</v>
       </c>
       <c r="C51" t="n">
-        <v>0.1348256824745072</v>
+        <v>0.138397285507785</v>
       </c>
       <c r="D51" t="n">
-        <v>0.5155452436194896</v>
+        <v>0.5078922934076138</v>
       </c>
       <c r="E51" t="n">
-        <v>0.5929368029739777</v>
+        <v>0.5343228200371057</v>
       </c>
     </row>
     <row r="52">
@@ -1315,16 +1315,16 @@
         <v>50</v>
       </c>
       <c r="B52" t="n">
-        <v>0.1369102018720963</v>
+        <v>0.1397086822373026</v>
       </c>
       <c r="C52" t="n">
-        <v>0.134787196914355</v>
+        <v>0.1382868281669087</v>
       </c>
       <c r="D52" t="n">
-        <v>0.505800464037123</v>
+        <v>0.5176415970287837</v>
       </c>
       <c r="E52" t="n">
-        <v>0.5892193308550185</v>
+        <v>0.5398886827458256</v>
       </c>
     </row>
     <row r="53">
@@ -1332,16 +1332,16 @@
         <v>51</v>
       </c>
       <c r="B53" t="n">
-        <v>0.1371937238556497</v>
+        <v>0.1402613454881836</v>
       </c>
       <c r="C53" t="n">
-        <v>0.1347314632601208</v>
+        <v>0.1382623116175334</v>
       </c>
       <c r="D53" t="n">
-        <v>0.505800464037123</v>
+        <v>0.5167130919220055</v>
       </c>
       <c r="E53" t="n">
-        <v>0.5910780669144982</v>
+        <v>0.5343228200371057</v>
       </c>
     </row>
     <row r="54">
@@ -1349,16 +1349,16 @@
         <v>52</v>
       </c>
       <c r="B54" t="n">
-        <v>0.1339682741638492</v>
+        <v>0.1397887365344693</v>
       </c>
       <c r="C54" t="n">
-        <v>0.1344941945539581</v>
+        <v>0.1383935726351208</v>
       </c>
       <c r="D54" t="n">
-        <v>0.5192575406032482</v>
+        <v>0.5259981429897864</v>
       </c>
       <c r="E54" t="n">
-        <v>0.5892193308550185</v>
+        <v>0.5361781076066791</v>
       </c>
     </row>
     <row r="55">
@@ -1366,16 +1366,16 @@
         <v>53</v>
       </c>
       <c r="B55" t="n">
-        <v>0.1339992376811364</v>
+        <v>0.1398175729109961</v>
       </c>
       <c r="C55" t="n">
-        <v>0.1339941802952025</v>
+        <v>0.1381275372372733</v>
       </c>
       <c r="D55" t="n">
-        <v>0.5211136890951276</v>
+        <v>0.5297121634168988</v>
       </c>
       <c r="E55" t="n">
-        <v>0.5892193308550185</v>
+        <v>0.5269016697588126</v>
       </c>
     </row>
     <row r="56">
@@ -1383,16 +1383,16 @@
         <v>54</v>
       </c>
       <c r="B56" t="n">
-        <v>0.1364136596812922</v>
+        <v>0.1398306464885964</v>
       </c>
       <c r="C56" t="n">
-        <v>0.1344518562157949</v>
+        <v>0.1376202586624357</v>
       </c>
       <c r="D56" t="n">
-        <v>0.5187935034802784</v>
+        <v>0.5171773444753947</v>
       </c>
       <c r="E56" t="n">
-        <v>0.5966542750929368</v>
+        <v>0.5528756957328386</v>
       </c>
     </row>
     <row r="57">
@@ -1400,16 +1400,16 @@
         <v>55</v>
       </c>
       <c r="B57" t="n">
-        <v>0.1365130832966636</v>
+        <v>0.1401269488474902</v>
       </c>
       <c r="C57" t="n">
-        <v>0.1344330600566334</v>
+        <v>0.1376514674888717</v>
       </c>
       <c r="D57" t="n">
-        <v>0.5136890951276102</v>
+        <v>0.521355617455896</v>
       </c>
       <c r="E57" t="n">
-        <v>0.5966542750929368</v>
+        <v>0.5417439703153989</v>
       </c>
     </row>
     <row r="58">
@@ -1417,16 +1417,16 @@
         <v>56</v>
       </c>
       <c r="B58" t="n">
-        <v>0.1351377304424258</v>
+        <v>0.1391824525507057</v>
       </c>
       <c r="C58" t="n">
-        <v>0.1336673373977343</v>
+        <v>0.1374875845180618</v>
       </c>
       <c r="D58" t="n">
-        <v>0.5243619489559165</v>
+        <v>0.5167130919220055</v>
       </c>
       <c r="E58" t="n">
-        <v>0.5929368029739777</v>
+        <v>0.549165120593692</v>
       </c>
     </row>
     <row r="59">
@@ -1434,16 +1434,16 @@
         <v>57</v>
       </c>
       <c r="B59" t="n">
-        <v>0.1347502474399174</v>
+        <v>0.1384028998367927</v>
       </c>
       <c r="C59" t="n">
-        <v>0.1342228005329768</v>
+        <v>0.1376532249980503</v>
       </c>
       <c r="D59" t="n">
-        <v>0.5201856148491879</v>
+        <v>0.5506035283194057</v>
       </c>
       <c r="E59" t="n">
-        <v>0.5929368029739777</v>
+        <v>0.5306122448979592</v>
       </c>
     </row>
     <row r="60">
@@ -1451,16 +1451,16 @@
         <v>58</v>
       </c>
       <c r="B60" t="n">
-        <v>0.1334998406031553</v>
+        <v>0.1402517274460372</v>
       </c>
       <c r="C60" t="n">
-        <v>0.1333752787775463</v>
+        <v>0.137603814403216</v>
       </c>
       <c r="D60" t="n">
-        <v>0.5271461716937355</v>
+        <v>0.5278551532033426</v>
       </c>
       <c r="E60" t="n">
-        <v>0.6003717472118959</v>
+        <v>0.5398886827458256</v>
       </c>
     </row>
     <row r="61">
@@ -1468,16 +1468,16 @@
         <v>59</v>
       </c>
       <c r="B61" t="n">
-        <v>0.1332606914288857</v>
+        <v>0.1382773281896816</v>
       </c>
       <c r="C61" t="n">
-        <v>0.1334638347228368</v>
+        <v>0.1375077093640963</v>
       </c>
       <c r="D61" t="n">
-        <v>0.5155452436194896</v>
+        <v>0.5366759517177344</v>
       </c>
       <c r="E61" t="n">
-        <v>0.5947955390334573</v>
+        <v>0.5435992578849722</v>
       </c>
     </row>
     <row r="62">
@@ -1485,16 +1485,16 @@
         <v>60</v>
       </c>
       <c r="B62" t="n">
-        <v>0.1340109510895084</v>
+        <v>0.1374554397428737</v>
       </c>
       <c r="C62" t="n">
-        <v>0.1336699773867925</v>
+        <v>0.1372616150312954</v>
       </c>
       <c r="D62" t="n">
-        <v>0.5155452436194896</v>
+        <v>0.531104921077066</v>
       </c>
       <c r="E62" t="n">
-        <v>0.6003717472118959</v>
+        <v>0.5473098330241187</v>
       </c>
     </row>
     <row r="63">
@@ -1502,16 +1502,16 @@
         <v>61</v>
       </c>
       <c r="B63" t="n">
-        <v>0.1348455276559381</v>
+        <v>0.1379362016039736</v>
       </c>
       <c r="C63" t="n">
-        <v>0.1330795221858554</v>
+        <v>0.1370544847514894</v>
       </c>
       <c r="D63" t="n">
-        <v>0.5160092807424594</v>
+        <v>0.5236768802228412</v>
       </c>
       <c r="E63" t="n">
-        <v>0.5985130111524164</v>
+        <v>0.5435992578849722</v>
       </c>
     </row>
     <row r="64">
@@ -1519,16 +1519,16 @@
         <v>62</v>
       </c>
       <c r="B64" t="n">
-        <v>0.1329270820407306</v>
+        <v>0.1353538965477663</v>
       </c>
       <c r="C64" t="n">
-        <v>0.1332859463161892</v>
+        <v>0.1372199356555939</v>
       </c>
       <c r="D64" t="n">
-        <v>0.5433874709976798</v>
+        <v>0.542711234911792</v>
       </c>
       <c r="E64" t="n">
-        <v>0.6059479553903345</v>
+        <v>0.5417439703153989</v>
       </c>
     </row>
     <row r="65">
@@ -1536,16 +1536,16 @@
         <v>63</v>
       </c>
       <c r="B65" t="n">
-        <v>0.1340477839112282</v>
+        <v>0.1352018705185722</v>
       </c>
       <c r="C65" t="n">
-        <v>0.1328544724318716</v>
+        <v>0.1369987461302015</v>
       </c>
       <c r="D65" t="n">
-        <v>0.5034802784222738</v>
+        <v>0.5445682451253482</v>
       </c>
       <c r="E65" t="n">
-        <v>0.6096654275092936</v>
+        <v>0.5473098330241187</v>
       </c>
     </row>
     <row r="66">
@@ -1553,16 +1553,16 @@
         <v>64</v>
       </c>
       <c r="B66" t="n">
-        <v>0.1319133525385576</v>
+        <v>0.1362087321193779</v>
       </c>
       <c r="C66" t="n">
-        <v>0.1335712075233459</v>
+        <v>0.1370860098136796</v>
       </c>
       <c r="D66" t="n">
-        <v>0.5359628770301624</v>
+        <v>0.5445682451253482</v>
       </c>
       <c r="E66" t="n">
-        <v>0.5892193308550185</v>
+        <v>0.5398886827458256</v>
       </c>
     </row>
     <row r="67">
@@ -1570,16 +1570,16 @@
         <v>65</v>
       </c>
       <c r="B67" t="n">
-        <v>0.1343277412302354</v>
+        <v>0.1357072740793228</v>
       </c>
       <c r="C67" t="n">
-        <v>0.1324521592921681</v>
+        <v>0.1368567215071784</v>
       </c>
       <c r="D67" t="n">
-        <v>0.5225058004640372</v>
+        <v>0.531569173630455</v>
       </c>
       <c r="E67" t="n">
-        <v>0.5985130111524164</v>
+        <v>0.5417439703153989</v>
       </c>
     </row>
     <row r="68">
@@ -1587,16 +1587,16 @@
         <v>66</v>
       </c>
       <c r="B68" t="n">
-        <v>0.1341576256296214</v>
+        <v>0.13726557046175</v>
       </c>
       <c r="C68" t="n">
-        <v>0.1322926473286417</v>
+        <v>0.1371496841311455</v>
       </c>
       <c r="D68" t="n">
-        <v>0.5252900232018561</v>
+        <v>0.5380687093779016</v>
       </c>
       <c r="E68" t="n">
-        <v>0.5985130111524164</v>
+        <v>0.5361781076066791</v>
       </c>
     </row>
     <row r="69">
@@ -1604,16 +1604,16 @@
         <v>67</v>
       </c>
       <c r="B69" t="n">
-        <v>0.1341235508375308</v>
+        <v>0.1373291716856115</v>
       </c>
       <c r="C69" t="n">
-        <v>0.1327131572696898</v>
+        <v>0.136928608847989</v>
       </c>
       <c r="D69" t="n">
-        <v>0.5336426914153132</v>
+        <v>0.5338904363974002</v>
       </c>
       <c r="E69" t="n">
-        <v>0.604089219330855</v>
+        <v>0.5435992578849722</v>
       </c>
     </row>
     <row r="70">
@@ -1621,16 +1621,16 @@
         <v>68</v>
       </c>
       <c r="B70" t="n">
-        <v>0.1320189603549593</v>
+        <v>0.1361629590392113</v>
       </c>
       <c r="C70" t="n">
-        <v>0.1327002189225621</v>
+        <v>0.1367424668537246</v>
       </c>
       <c r="D70" t="n">
-        <v>0.5303944315545244</v>
+        <v>0.5348189415041783</v>
       </c>
       <c r="E70" t="n">
-        <v>0.6022304832713755</v>
+        <v>0.5417439703153989</v>
       </c>
     </row>
     <row r="71">
@@ -1638,16 +1638,16 @@
         <v>69</v>
       </c>
       <c r="B71" t="n">
-        <v>0.1330607859965633</v>
+        <v>0.1350661408813561</v>
       </c>
       <c r="C71" t="n">
-        <v>0.132630983988444</v>
+        <v>0.136657554242346</v>
       </c>
       <c r="D71" t="n">
-        <v>0.5406032482598608</v>
+        <v>0.5454967502321263</v>
       </c>
       <c r="E71" t="n">
-        <v>0.5947955390334573</v>
+        <v>0.5435992578849722</v>
       </c>
     </row>
     <row r="72">
@@ -1655,16 +1655,16 @@
         <v>70</v>
       </c>
       <c r="B72" t="n">
-        <v>0.132524719571366</v>
+        <v>0.1358139644212583</v>
       </c>
       <c r="C72" t="n">
-        <v>0.133057527244091</v>
+        <v>0.136981708308061</v>
       </c>
       <c r="D72" t="n">
-        <v>0.5378190255220417</v>
+        <v>0.5352831940575673</v>
       </c>
       <c r="E72" t="n">
-        <v>0.6078066914498141</v>
+        <v>0.5454545454545454</v>
       </c>
     </row>
     <row r="73">
@@ -1672,16 +1672,16 @@
         <v>71</v>
       </c>
       <c r="B73" t="n">
-        <v>0.1321738180430496</v>
+        <v>0.135477703941219</v>
       </c>
       <c r="C73" t="n">
-        <v>0.1324806693527434</v>
+        <v>0.1366686738199658</v>
       </c>
       <c r="D73" t="n">
-        <v>0.5252900232018561</v>
+        <v>0.5547818012999072</v>
       </c>
       <c r="E73" t="n">
-        <v>0.604089219330855</v>
+        <v>0.5435992578849722</v>
       </c>
     </row>
     <row r="74">
@@ -1689,16 +1689,16 @@
         <v>72</v>
       </c>
       <c r="B74" t="n">
-        <v>0.132151401218246</v>
+        <v>0.1369434783563894</v>
       </c>
       <c r="C74" t="n">
-        <v>0.1324985085262192</v>
+        <v>0.1362573876976967</v>
       </c>
       <c r="D74" t="n">
-        <v>0.5285382830626451</v>
+        <v>0.5362116991643454</v>
       </c>
       <c r="E74" t="n">
-        <v>0.604089219330855</v>
+        <v>0.5510204081632653</v>
       </c>
     </row>
     <row r="75">
@@ -1706,16 +1706,16 @@
         <v>73</v>
       </c>
       <c r="B75" t="n">
-        <v>0.1309201410588096</v>
+        <v>0.1358340792357922</v>
       </c>
       <c r="C75" t="n">
-        <v>0.1322542395856645</v>
+        <v>0.1364700082275603</v>
       </c>
       <c r="D75" t="n">
-        <v>0.5438515081206496</v>
+        <v>0.5478180129990715</v>
       </c>
       <c r="E75" t="n">
-        <v>0.604089219330855</v>
+        <v>0.5510204081632653</v>
       </c>
     </row>
     <row r="76">
@@ -1723,16 +1723,16 @@
         <v>74</v>
       </c>
       <c r="B76" t="n">
-        <v>0.1318805579315214</v>
+        <v>0.1359658780343392</v>
       </c>
       <c r="C76" t="n">
-        <v>0.1318742061654727</v>
+        <v>0.1363439667556021</v>
       </c>
       <c r="D76" t="n">
-        <v>0.5373549883990719</v>
+        <v>0.5376044568245125</v>
       </c>
       <c r="E76" t="n">
-        <v>0.604089219330855</v>
+        <v>0.5473098330241187</v>
       </c>
     </row>
     <row r="77">
@@ -1740,16 +1740,16 @@
         <v>75</v>
       </c>
       <c r="B77" t="n">
-        <v>0.1312402640195454</v>
+        <v>0.13625918372589</v>
       </c>
       <c r="C77" t="n">
-        <v>0.1316230388151275</v>
+        <v>0.1359874217046632</v>
       </c>
       <c r="D77" t="n">
-        <v>0.5531322505800464</v>
+        <v>0.5482822655524605</v>
       </c>
       <c r="E77" t="n">
-        <v>0.6059479553903345</v>
+        <v>0.5528756957328386</v>
       </c>
     </row>
     <row r="78">
@@ -1757,16 +1757,16 @@
         <v>76</v>
       </c>
       <c r="B78" t="n">
-        <v>0.1305212139645044</v>
+        <v>0.133358549545793</v>
       </c>
       <c r="C78" t="n">
-        <v>0.1315073263314035</v>
+        <v>0.1361204261581103</v>
       </c>
       <c r="D78" t="n">
-        <v>0.5559164733178654</v>
+        <v>0.5515320334261838</v>
       </c>
       <c r="E78" t="n">
-        <v>0.604089219330855</v>
+        <v>0.5454545454545454</v>
       </c>
     </row>
     <row r="79">
@@ -1774,16 +1774,16 @@
         <v>77</v>
       </c>
       <c r="B79" t="n">
-        <v>0.1312331020393792</v>
+        <v>0.1347960693871274</v>
       </c>
       <c r="C79" t="n">
-        <v>0.1320689982838101</v>
+        <v>0.1364322478572527</v>
       </c>
       <c r="D79" t="n">
-        <v>0.5494199535962877</v>
+        <v>0.5571030640668524</v>
       </c>
       <c r="E79" t="n">
-        <v>0.6059479553903345</v>
+        <v>0.5454545454545454</v>
       </c>
     </row>
     <row r="80">
@@ -1791,16 +1791,16 @@
         <v>78</v>
       </c>
       <c r="B80" t="n">
-        <v>0.1303969198728309</v>
+        <v>0.1343971872154404</v>
       </c>
       <c r="C80" t="n">
-        <v>0.132053688996368</v>
+        <v>0.1367101677589946</v>
       </c>
       <c r="D80" t="n">
-        <v>0.5303944315545244</v>
+        <v>0.5584958217270195</v>
       </c>
       <c r="E80" t="n">
-        <v>0.6078066914498141</v>
+        <v>0.5435992578849722</v>
       </c>
     </row>
     <row r="81">
@@ -1808,16 +1808,16 @@
         <v>79</v>
       </c>
       <c r="B81" t="n">
-        <v>0.1314960220719085</v>
+        <v>0.1347968170748037</v>
       </c>
       <c r="C81" t="n">
-        <v>0.1322512287232611</v>
+        <v>0.1357606773575147</v>
       </c>
       <c r="D81" t="n">
-        <v>0.5364269141531323</v>
+        <v>0.5598885793871866</v>
       </c>
       <c r="E81" t="n">
-        <v>0.6115241635687733</v>
+        <v>0.5510204081632653</v>
       </c>
     </row>
     <row r="82">
@@ -1825,16 +1825,16 @@
         <v>80</v>
       </c>
       <c r="B82" t="n">
-        <v>0.1302621268174227</v>
+        <v>0.134632260483854</v>
       </c>
       <c r="C82" t="n">
-        <v>0.1313123189740711</v>
+        <v>0.1360284644696448</v>
       </c>
       <c r="D82" t="n">
-        <v>0.5498839907192575</v>
+        <v>0.5608170844939647</v>
       </c>
       <c r="E82" t="n">
-        <v>0.6078066914498141</v>
+        <v>0.5473098330241187</v>
       </c>
     </row>
     <row r="83">
@@ -1842,16 +1842,16 @@
         <v>81</v>
       </c>
       <c r="B83" t="n">
-        <v>0.1305349357426167</v>
+        <v>0.1334864306537544</v>
       </c>
       <c r="C83" t="n">
-        <v>0.1313418423136075</v>
+        <v>0.1358429110712475</v>
       </c>
       <c r="D83" t="n">
-        <v>0.5531322505800464</v>
+        <v>0.5408542246982359</v>
       </c>
       <c r="E83" t="n">
-        <v>0.5985130111524164</v>
+        <v>0.5473098330241187</v>
       </c>
     </row>
     <row r="84">
@@ -1859,16 +1859,16 @@
         <v>82</v>
       </c>
       <c r="B84" t="n">
-        <v>0.1306942578624277</v>
+        <v>0.1336880192598876</v>
       </c>
       <c r="C84" t="n">
-        <v>0.1316240173247125</v>
+        <v>0.1359126857585377</v>
       </c>
       <c r="D84" t="n">
-        <v>0.5317865429234339</v>
+        <v>0.5538532961931291</v>
       </c>
       <c r="E84" t="n">
-        <v>0.6022304832713755</v>
+        <v>0.5473098330241187</v>
       </c>
     </row>
     <row r="85">
@@ -1876,16 +1876,16 @@
         <v>83</v>
       </c>
       <c r="B85" t="n">
-        <v>0.1294214521699092</v>
+        <v>0.1337412271429511</v>
       </c>
       <c r="C85" t="n">
-        <v>0.1308497107691235</v>
+        <v>0.1361137396759457</v>
       </c>
       <c r="D85" t="n">
-        <v>0.5498839907192575</v>
+        <v>0.5557103064066853</v>
       </c>
       <c r="E85" t="n">
-        <v>0.6022304832713755</v>
+        <v>0.5454545454545454</v>
       </c>
     </row>
     <row r="86">
@@ -1893,16 +1893,16 @@
         <v>84</v>
       </c>
       <c r="B86" t="n">
-        <v>0.1308136832188158</v>
+        <v>0.1325666873770601</v>
       </c>
       <c r="C86" t="n">
-        <v>0.1310150888231066</v>
+        <v>0.135739697350396</v>
       </c>
       <c r="D86" t="n">
-        <v>0.5461716937354988</v>
+        <v>0.5482822655524605</v>
       </c>
       <c r="E86" t="n">
-        <v>0.604089219330855</v>
+        <v>0.5361781076066791</v>
       </c>
     </row>
     <row r="87">
@@ -1910,16 +1910,16 @@
         <v>85</v>
       </c>
       <c r="B87" t="n">
-        <v>0.1307242819491555</v>
+        <v>0.1333896116737057</v>
       </c>
       <c r="C87" t="n">
-        <v>0.1310624364349577</v>
+        <v>0.1351226816574732</v>
       </c>
       <c r="D87" t="n">
-        <v>0.5545243619489559</v>
+        <v>0.5673166202414113</v>
       </c>
       <c r="E87" t="n">
-        <v>0.604089219330855</v>
+        <v>0.5528756957328386</v>
       </c>
     </row>
     <row r="88">
@@ -1927,16 +1927,16 @@
         <v>86</v>
       </c>
       <c r="B88" t="n">
-        <v>0.1304837265873657</v>
+        <v>0.133589613087037</v>
       </c>
       <c r="C88" t="n">
-        <v>0.1309684365987778</v>
+        <v>0.135583666463693</v>
       </c>
       <c r="D88" t="n">
-        <v>0.5447795823665893</v>
+        <v>0.5571030640668524</v>
       </c>
       <c r="E88" t="n">
-        <v>0.6078066914498141</v>
+        <v>0.5435992578849722</v>
       </c>
     </row>
     <row r="89">
@@ -1944,16 +1944,16 @@
         <v>87</v>
       </c>
       <c r="B89" t="n">
-        <v>0.1284381602616871</v>
+        <v>0.1324247831807417</v>
       </c>
       <c r="C89" t="n">
-        <v>0.1308460798528459</v>
+        <v>0.1351047390037113</v>
       </c>
       <c r="D89" t="n">
-        <v>0.5614849187935035</v>
+        <v>0.5608170844939647</v>
       </c>
       <c r="E89" t="n">
-        <v>0.6115241635687733</v>
+        <v>0.5602968460111317</v>
       </c>
     </row>
     <row r="90">
@@ -1961,16 +1961,16 @@
         <v>88</v>
       </c>
       <c r="B90" t="n">
-        <v>0.1287121069343651</v>
+        <v>0.1335100159049034</v>
       </c>
       <c r="C90" t="n">
-        <v>0.1301195389694638</v>
+        <v>0.1355628305011325</v>
       </c>
       <c r="D90" t="n">
-        <v>0.5693735498839907</v>
+        <v>0.552924791086351</v>
       </c>
       <c r="E90" t="n">
-        <v>0.6096654275092936</v>
+        <v>0.5454545454545454</v>
       </c>
     </row>
     <row r="91">
@@ -1978,16 +1978,16 @@
         <v>89</v>
       </c>
       <c r="B91" t="n">
-        <v>0.1308851513792487</v>
+        <v>0.1322162878863952</v>
       </c>
       <c r="C91" t="n">
-        <v>0.1306249863571591</v>
+        <v>0.1352483688129319</v>
       </c>
       <c r="D91" t="n">
-        <v>0.5498839907192575</v>
+        <v>0.5636025998142989</v>
       </c>
       <c r="E91" t="n">
-        <v>0.604089219330855</v>
+        <v>0.5528756957328386</v>
       </c>
     </row>
     <row r="92">
@@ -1995,16 +1995,16 @@
         <v>90</v>
       </c>
       <c r="B92" t="n">
-        <v>0.1292984244578025</v>
+        <v>0.1321170362917816</v>
       </c>
       <c r="C92" t="n">
-        <v>0.13065222154061</v>
+        <v>0.1350033995178011</v>
       </c>
       <c r="D92" t="n">
-        <v>0.5605568445475638</v>
+        <v>0.5575673166202414</v>
       </c>
       <c r="E92" t="n">
-        <v>0.6133828996282528</v>
+        <v>0.5584415584415584</v>
       </c>
     </row>
     <row r="93">
@@ -2012,16 +2012,16 @@
         <v>91</v>
       </c>
       <c r="B93" t="n">
-        <v>0.1283556266742594</v>
+        <v>0.1319501921534538</v>
       </c>
       <c r="C93" t="n">
-        <v>0.1303957750399908</v>
+        <v>0.1354560802380244</v>
       </c>
       <c r="D93" t="n">
-        <v>0.568445475638051</v>
+        <v>0.5668523676880223</v>
       </c>
       <c r="E93" t="n">
-        <v>0.6133828996282528</v>
+        <v>0.5454545454545454</v>
       </c>
     </row>
     <row r="94">
@@ -2029,16 +2029,16 @@
         <v>92</v>
       </c>
       <c r="B94" t="n">
-        <v>0.1298609472372953</v>
+        <v>0.1322755901252522</v>
       </c>
       <c r="C94" t="n">
-        <v>0.1307875232564079</v>
+        <v>0.1350777629348967</v>
       </c>
       <c r="D94" t="n">
-        <v>0.548491879350348</v>
+        <v>0.5636025998142989</v>
       </c>
       <c r="E94" t="n">
-        <v>0.6059479553903345</v>
+        <v>0.5510204081632653</v>
       </c>
     </row>
     <row r="95">
@@ -2046,16 +2046,16 @@
         <v>93</v>
       </c>
       <c r="B95" t="n">
-        <v>0.127928620971301</v>
+        <v>0.1323033369639341</v>
       </c>
       <c r="C95" t="n">
-        <v>0.1309223522742589</v>
+        <v>0.1351781710982323</v>
       </c>
       <c r="D95" t="n">
-        <v>0.5545243619489559</v>
+        <v>0.5575673166202414</v>
       </c>
       <c r="E95" t="n">
-        <v>0.6059479553903345</v>
+        <v>0.5528756957328386</v>
       </c>
     </row>
     <row r="96">
@@ -2063,16 +2063,16 @@
         <v>94</v>
       </c>
       <c r="B96" t="n">
-        <v>0.1285746599383214</v>
+        <v>0.1317065730690956</v>
       </c>
       <c r="C96" t="n">
-        <v>0.1304567000932164</v>
+        <v>0.1351888014210595</v>
       </c>
       <c r="D96" t="n">
-        <v>0.5624129930394431</v>
+        <v>0.5668523676880223</v>
       </c>
       <c r="E96" t="n">
-        <v>0.6133828996282528</v>
+        <v>0.5547309833024119</v>
       </c>
     </row>
     <row r="97">
@@ -2080,16 +2080,16 @@
         <v>95</v>
       </c>
       <c r="B97" t="n">
-        <v>0.1284691908341997</v>
+        <v>0.131706602871418</v>
       </c>
       <c r="C97" t="n">
-        <v>0.1306193760699696</v>
+        <v>0.1349901838435067</v>
       </c>
       <c r="D97" t="n">
-        <v>0.5656612529002321</v>
+        <v>0.5552460538532962</v>
       </c>
       <c r="E97" t="n">
-        <v>0.6115241635687733</v>
+        <v>0.549165120593692</v>
       </c>
     </row>
     <row r="98">
@@ -2097,16 +2097,16 @@
         <v>96</v>
       </c>
       <c r="B98" t="n">
-        <v>0.1287412365131518</v>
+        <v>0.1313608922064304</v>
       </c>
       <c r="C98" t="n">
-        <v>0.1299396231770515</v>
+        <v>0.1347910546594196</v>
       </c>
       <c r="D98" t="n">
-        <v>0.5577726218097447</v>
+        <v>0.5687093779015785</v>
       </c>
       <c r="E98" t="n">
-        <v>0.6133828996282528</v>
+        <v>0.5454545454545454</v>
       </c>
     </row>
     <row r="99">
@@ -2114,16 +2114,16 @@
         <v>97</v>
       </c>
       <c r="B99" t="n">
-        <v>0.1278308976222487</v>
+        <v>0.1331852786242962</v>
       </c>
       <c r="C99" t="n">
-        <v>0.1302302877108256</v>
+        <v>0.1355326821406682</v>
       </c>
       <c r="D99" t="n">
-        <v>0.5577726218097447</v>
+        <v>0.5436397400185701</v>
       </c>
       <c r="E99" t="n">
-        <v>0.6115241635687733</v>
+        <v>0.5473098330241187</v>
       </c>
     </row>
     <row r="100">
@@ -2131,16 +2131,16 @@
         <v>98</v>
       </c>
       <c r="B100" t="n">
-        <v>0.1281958180753624</v>
+        <v>0.1330778688630637</v>
       </c>
       <c r="C100" t="n">
-        <v>0.1300371173355314</v>
+        <v>0.1350169546074337</v>
       </c>
       <c r="D100" t="n">
-        <v>0.5638051044083526</v>
+        <v>0.5594243268337976</v>
       </c>
       <c r="E100" t="n">
-        <v>0.6152416356877324</v>
+        <v>0.5473098330241187</v>
       </c>
     </row>
     <row r="101">
@@ -2148,16 +2148,16 @@
         <v>99</v>
       </c>
       <c r="B101" t="n">
-        <v>0.1275648779290564</v>
+        <v>0.13129868467941</v>
       </c>
       <c r="C101" t="n">
-        <v>0.1291302699181769</v>
+        <v>0.1350934993889597</v>
       </c>
       <c r="D101" t="n">
-        <v>0.5698375870069605</v>
+        <v>0.5766016713091922</v>
       </c>
       <c r="E101" t="n">
-        <v>0.6133828996282528</v>
+        <v>0.5454545454545454</v>
       </c>
     </row>
     <row r="102">
@@ -2165,16 +2165,16 @@
         <v>100</v>
       </c>
       <c r="B102" t="n">
-        <v>0.1275663136997644</v>
+        <v>0.1303638101500623</v>
       </c>
       <c r="C102" t="n">
-        <v>0.129068474802706</v>
+        <v>0.135550893843174</v>
       </c>
       <c r="D102" t="n">
-        <v>0.5624129930394431</v>
+        <v>0.5714948932219127</v>
       </c>
       <c r="E102" t="n">
-        <v>0.6152416356877324</v>
+        <v>0.5417439703153989</v>
       </c>
     </row>
     <row r="103">
@@ -2182,16 +2182,16 @@
         <v>101</v>
       </c>
       <c r="B103" t="n">
-        <v>0.1273609597016783</v>
+        <v>0.130552881561658</v>
       </c>
       <c r="C103" t="n">
-        <v>0.1286249897546238</v>
+        <v>0.135099235508177</v>
       </c>
       <c r="D103" t="n">
-        <v>0.5494199535962877</v>
+        <v>0.5724233983286908</v>
       </c>
       <c r="E103" t="n">
-        <v>0.604089219330855</v>
+        <v>0.5435992578849722</v>
       </c>
     </row>
     <row r="104">
@@ -2199,16 +2199,16 @@
         <v>102</v>
       </c>
       <c r="B104" t="n">
-        <v>0.1269615367054939</v>
+        <v>0.131432856707012</v>
       </c>
       <c r="C104" t="n">
-        <v>0.1294140981303321</v>
+        <v>0.1347511369321081</v>
       </c>
       <c r="D104" t="n">
-        <v>0.5679814385150812</v>
+        <v>0.5622098421541318</v>
       </c>
       <c r="E104" t="n">
-        <v>0.6133828996282528</v>
+        <v>0.5547309833024119</v>
       </c>
     </row>
     <row r="105">
@@ -2216,16 +2216,16 @@
         <v>103</v>
       </c>
       <c r="B105" t="n">
-        <v>0.1269378629239167</v>
+        <v>0.1291371128138374</v>
       </c>
       <c r="C105" t="n">
-        <v>0.1295089407099618</v>
+        <v>0.1351508233282301</v>
       </c>
       <c r="D105" t="n">
-        <v>0.5661252900232019</v>
+        <v>0.5807799442896936</v>
       </c>
       <c r="E105" t="n">
-        <v>0.6059479553903345</v>
+        <v>0.5361781076066791</v>
       </c>
     </row>
     <row r="106">
@@ -2233,16 +2233,16 @@
         <v>104</v>
       </c>
       <c r="B106" t="n">
-        <v>0.1255886896568186</v>
+        <v>0.1310934345511829</v>
       </c>
       <c r="C106" t="n">
-        <v>0.1290702993671099</v>
+        <v>0.1348156150844362</v>
       </c>
       <c r="D106" t="n">
-        <v>0.5758700696055684</v>
+        <v>0.5598885793871866</v>
       </c>
       <c r="E106" t="n">
-        <v>0.5985130111524164</v>
+        <v>0.5398886827458256</v>
       </c>
     </row>
     <row r="107">
@@ -2250,16 +2250,16 @@
         <v>105</v>
       </c>
       <c r="B107" t="n">
-        <v>0.1261137005160837</v>
+        <v>0.1286472564234453</v>
       </c>
       <c r="C107" t="n">
-        <v>0.1289564735359616</v>
+        <v>0.1352286098731889</v>
       </c>
       <c r="D107" t="n">
-        <v>0.5573085846867749</v>
+        <v>0.584958217270195</v>
       </c>
       <c r="E107" t="n">
-        <v>0.604089219330855</v>
+        <v>0.5361781076066791</v>
       </c>
     </row>
     <row r="108">
@@ -2267,16 +2267,16 @@
         <v>106</v>
       </c>
       <c r="B108" t="n">
-        <v>0.1266571581363678</v>
+        <v>0.1301193015978617</v>
       </c>
       <c r="C108" t="n">
-        <v>0.1287786546680662</v>
+        <v>0.1346595187981924</v>
       </c>
       <c r="D108" t="n">
-        <v>0.5744779582366589</v>
+        <v>0.5701021355617456</v>
       </c>
       <c r="E108" t="n">
-        <v>0.6115241635687733</v>
+        <v>0.549165120593692</v>
       </c>
     </row>
     <row r="109">
@@ -2284,16 +2284,16 @@
         <v>107</v>
       </c>
       <c r="B109" t="n">
-        <v>0.1259159309899106</v>
+        <v>0.1293815448880196</v>
       </c>
       <c r="C109" t="n">
-        <v>0.1287382104330593</v>
+        <v>0.1349606745772892</v>
       </c>
       <c r="D109" t="n">
-        <v>0.5531322505800464</v>
+        <v>0.5608170844939647</v>
       </c>
       <c r="E109" t="n">
-        <v>0.6096654275092936</v>
+        <v>0.5454545454545454</v>
       </c>
     </row>
     <row r="110">
@@ -2301,16 +2301,16 @@
         <v>108</v>
       </c>
       <c r="B110" t="n">
-        <v>0.1262488608412883</v>
+        <v>0.1279358664417968</v>
       </c>
       <c r="C110" t="n">
-        <v>0.1289521679282188</v>
+        <v>0.1349230292770598</v>
       </c>
       <c r="D110" t="n">
-        <v>0.5763341067285382</v>
+        <v>0.5766016713091922</v>
       </c>
       <c r="E110" t="n">
-        <v>0.6115241635687733</v>
+        <v>0.5435992578849722</v>
       </c>
     </row>
     <row r="111">
@@ -2318,16 +2318,16 @@
         <v>109</v>
       </c>
       <c r="B111" t="n">
-        <v>0.1263415589928627</v>
+        <v>0.1290747269111521</v>
       </c>
       <c r="C111" t="n">
-        <v>0.1287063890033298</v>
+        <v>0.1343315127823088</v>
       </c>
       <c r="D111" t="n">
-        <v>0.5679814385150812</v>
+        <v>0.585886722376973</v>
       </c>
       <c r="E111" t="n">
-        <v>0.6022304832713755</v>
+        <v>0.5473098330241187</v>
       </c>
     </row>
     <row r="112">
@@ -2335,16 +2335,16 @@
         <v>110</v>
       </c>
       <c r="B112" t="n">
-        <v>0.1247188192518318</v>
+        <v>0.1300662898403757</v>
       </c>
       <c r="C112" t="n">
-        <v>0.1288290296991666</v>
+        <v>0.1347082017196549</v>
       </c>
       <c r="D112" t="n">
-        <v>0.5698375870069605</v>
+        <v>0.5724233983286908</v>
       </c>
       <c r="E112" t="n">
-        <v>0.5985130111524164</v>
+        <v>0.5473098330241187</v>
       </c>
     </row>
     <row r="113">
@@ -2352,16 +2352,16 @@
         <v>111</v>
       </c>
       <c r="B113" t="n">
-        <v>0.1258007158689639</v>
+        <v>0.1278986720477834</v>
       </c>
       <c r="C113" t="n">
-        <v>0.128435658911864</v>
+        <v>0.135035833550824</v>
       </c>
       <c r="D113" t="n">
-        <v>0.5587006960556845</v>
+        <v>0.5714948932219127</v>
       </c>
       <c r="E113" t="n">
-        <v>0.604089219330855</v>
+        <v>0.5398886827458256</v>
       </c>
     </row>
     <row r="114">
@@ -2369,16 +2369,16 @@
         <v>112</v>
       </c>
       <c r="B114" t="n">
-        <v>0.12533765045159</v>
+        <v>0.1279215089538518</v>
       </c>
       <c r="C114" t="n">
-        <v>0.1287057275573412</v>
+        <v>0.1348138716485765</v>
       </c>
       <c r="D114" t="n">
-        <v>0.5781902552204177</v>
+        <v>0.575208913649025</v>
       </c>
       <c r="E114" t="n">
-        <v>0.604089219330855</v>
+        <v>0.5454545454545454</v>
       </c>
     </row>
     <row r="115">
@@ -2386,16 +2386,16 @@
         <v>113</v>
       </c>
       <c r="B115" t="n">
-        <v>0.1250539989594151</v>
+        <v>0.1316428653457586</v>
       </c>
       <c r="C115" t="n">
-        <v>0.1286532754699389</v>
+        <v>0.1352746668789122</v>
       </c>
       <c r="D115" t="n">
-        <v>0.5679814385150812</v>
+        <v>0.5571030640668524</v>
       </c>
       <c r="E115" t="n">
-        <v>0.5966542750929368</v>
+        <v>0.5435992578849722</v>
       </c>
     </row>
     <row r="116">
@@ -2403,16 +2403,16 @@
         <v>114</v>
       </c>
       <c r="B116" t="n">
-        <v>0.125150908880374</v>
+        <v>0.1276250810307615</v>
       </c>
       <c r="C116" t="n">
-        <v>0.1287131160497665</v>
+        <v>0.1345825708574719</v>
       </c>
       <c r="D116" t="n">
-        <v>0.568445475638051</v>
+        <v>0.5803156917363046</v>
       </c>
       <c r="E116" t="n">
-        <v>0.604089219330855</v>
+        <v>0.5510204081632653</v>
       </c>
     </row>
     <row r="117">
@@ -2420,16 +2420,16 @@
         <v>115</v>
       </c>
       <c r="B117" t="n">
-        <v>0.1252054670716033</v>
+        <v>0.1294218895628172</v>
       </c>
       <c r="C117" t="n">
-        <v>0.1286923984686534</v>
+        <v>0.1347851165466838</v>
       </c>
       <c r="D117" t="n">
-        <v>0.5740139211136891</v>
+        <v>0.5770659238625813</v>
       </c>
       <c r="E117" t="n">
-        <v>0.5985130111524164</v>
+        <v>0.5473098330241187</v>
       </c>
     </row>
     <row r="118">
@@ -2437,16 +2437,16 @@
         <v>116</v>
       </c>
       <c r="B118" t="n">
-        <v>0.12593683381291</v>
+        <v>0.1281691778670339</v>
       </c>
       <c r="C118" t="n">
-        <v>0.1283787356482612</v>
+        <v>0.1344233676791191</v>
       </c>
       <c r="D118" t="n">
-        <v>0.5749419953596288</v>
+        <v>0.5668523676880223</v>
       </c>
       <c r="E118" t="n">
-        <v>0.5966542750929368</v>
+        <v>0.549165120593692</v>
       </c>
     </row>
     <row r="119">
@@ -2454,16 +2454,16 @@
         <v>117</v>
       </c>
       <c r="B119" t="n">
-        <v>0.1235541990574668</v>
+        <v>0.1286984162733835</v>
       </c>
       <c r="C119" t="n">
-        <v>0.1275731714235412</v>
+        <v>0.1349716261029243</v>
       </c>
       <c r="D119" t="n">
-        <v>0.5703016241299304</v>
+        <v>0.5696378830083565</v>
       </c>
       <c r="E119" t="n">
-        <v>0.604089219330855</v>
+        <v>0.5435992578849722</v>
       </c>
     </row>
     <row r="120">
@@ -2471,16 +2471,16 @@
         <v>118</v>
       </c>
       <c r="B120" t="n">
-        <v>0.1264383514576098</v>
+        <v>0.1281635138918372</v>
       </c>
       <c r="C120" t="n">
-        <v>0.1276306096050474</v>
+        <v>0.1344277767671479</v>
       </c>
       <c r="D120" t="n">
-        <v>0.5647331786542923</v>
+        <v>0.5738161559888579</v>
       </c>
       <c r="E120" t="n">
-        <v>0.6003717472118959</v>
+        <v>0.549165120593692</v>
       </c>
     </row>
     <row r="121">
@@ -2488,16 +2488,16 @@
         <v>119</v>
       </c>
       <c r="B121" t="n">
-        <v>0.1249443312339923</v>
+        <v>0.1287906693623346</v>
       </c>
       <c r="C121" t="n">
-        <v>0.1279975482159191</v>
+        <v>0.1346027246779866</v>
       </c>
       <c r="D121" t="n">
-        <v>0.5651972157772622</v>
+        <v>0.5789229340761374</v>
       </c>
       <c r="E121" t="n">
-        <v>0.6003717472118959</v>
+        <v>0.549165120593692</v>
       </c>
     </row>
     <row r="122">
@@ -2505,16 +2505,16 @@
         <v>120</v>
       </c>
       <c r="B122" t="n">
-        <v>0.1245056403910413</v>
+        <v>0.1277944964959341</v>
       </c>
       <c r="C122" t="n">
-        <v>0.127717605067624</v>
+        <v>0.1349670506185955</v>
       </c>
       <c r="D122" t="n">
-        <v>0.5814385150812065</v>
+        <v>0.5812441968430826</v>
       </c>
       <c r="E122" t="n">
-        <v>0.5929368029739777</v>
+        <v>0.549165120593692</v>
       </c>
     </row>
     <row r="123">
@@ -2522,16 +2522,16 @@
         <v>121</v>
       </c>
       <c r="B123" t="n">
-        <v>0.1253737921223921</v>
+        <v>0.12746893263915</v>
       </c>
       <c r="C123" t="n">
-        <v>0.1277576237916946</v>
+        <v>0.134431724747022</v>
       </c>
       <c r="D123" t="n">
-        <v>0.5851508120649652</v>
+        <v>0.5779944289693594</v>
       </c>
       <c r="E123" t="n">
-        <v>0.6003717472118959</v>
+        <v>0.5528756957328386</v>
       </c>
     </row>
     <row r="124">
@@ -2539,16 +2539,16 @@
         <v>122</v>
       </c>
       <c r="B124" t="n">
-        <v>0.1227622319232015</v>
+        <v>0.1279081036062802</v>
       </c>
       <c r="C124" t="n">
-        <v>0.1279560137126181</v>
+        <v>0.1347689007719358</v>
       </c>
       <c r="D124" t="n">
-        <v>0.6023201856148492</v>
+        <v>0.5821727019498607</v>
       </c>
       <c r="E124" t="n">
-        <v>0.6059479553903345</v>
+        <v>0.5528756957328386</v>
       </c>
     </row>
     <row r="125">
@@ -2556,16 +2556,16 @@
         <v>123</v>
       </c>
       <c r="B125" t="n">
-        <v>0.1245873537571991</v>
+        <v>0.1284294779248097</v>
       </c>
       <c r="C125" t="n">
-        <v>0.1283197411232525</v>
+        <v>0.1349905191196336</v>
       </c>
       <c r="D125" t="n">
-        <v>0.5740139211136891</v>
+        <v>0.5756731662024142</v>
       </c>
       <c r="E125" t="n">
-        <v>0.604089219330855</v>
+        <v>0.5454545454545454</v>
       </c>
     </row>
     <row r="126">
@@ -2573,16 +2573,16 @@
         <v>124</v>
       </c>
       <c r="B126" t="n">
-        <v>0.1245453221833005</v>
+        <v>0.1273655448766316</v>
       </c>
       <c r="C126" t="n">
-        <v>0.1280964803364542</v>
+        <v>0.1345964438385434</v>
       </c>
       <c r="D126" t="n">
-        <v>0.5614849187935035</v>
+        <v>0.5775301764159703</v>
       </c>
       <c r="E126" t="n">
-        <v>0.5929368029739777</v>
+        <v>0.5584415584415584</v>
       </c>
     </row>
     <row r="127">
@@ -2590,16 +2590,16 @@
         <v>125</v>
       </c>
       <c r="B127" t="n">
-        <v>0.1232581480461008</v>
+        <v>0.1280156198669882</v>
       </c>
       <c r="C127" t="n">
-        <v>0.1274830169147915</v>
+        <v>0.1341955463091532</v>
       </c>
       <c r="D127" t="n">
-        <v>0.5781902552204177</v>
+        <v>0.5761374187558032</v>
       </c>
       <c r="E127" t="n">
-        <v>0.5966542750929368</v>
+        <v>0.5528756957328386</v>
       </c>
     </row>
     <row r="128">
@@ -2607,16 +2607,16 @@
         <v>126</v>
       </c>
       <c r="B128" t="n">
-        <v>0.1256000640637734</v>
+        <v>0.1257399984580629</v>
       </c>
       <c r="C128" t="n">
-        <v>0.1277562023864852</v>
+        <v>0.1343225265542666</v>
       </c>
       <c r="D128" t="n">
-        <v>0.582830626450116</v>
+        <v>0.596100278551532</v>
       </c>
       <c r="E128" t="n">
-        <v>0.5966542750929368</v>
+        <v>0.5528756957328386</v>
       </c>
     </row>
     <row r="129">
@@ -2624,16 +2624,16 @@
         <v>127</v>
       </c>
       <c r="B129" t="n">
-        <v>0.1232995982555782</v>
+        <v>0.1265749041648472</v>
       </c>
       <c r="C129" t="n">
-        <v>0.1279884725809097</v>
+        <v>0.1343856602907181</v>
       </c>
       <c r="D129" t="n">
-        <v>0.5832946635730858</v>
+        <v>0.5896007428040855</v>
       </c>
       <c r="E129" t="n">
-        <v>0.6003717472118959</v>
+        <v>0.5528756957328386</v>
       </c>
     </row>
     <row r="130">
@@ -2641,16 +2641,16 @@
         <v>128</v>
       </c>
       <c r="B130" t="n">
-        <v>0.1237279667573817</v>
+        <v>0.1273713313481387</v>
       </c>
       <c r="C130" t="n">
-        <v>0.1281983430186907</v>
+        <v>0.1344325757688946</v>
       </c>
       <c r="D130" t="n">
-        <v>0.5846867749419954</v>
+        <v>0.585422469823584</v>
       </c>
       <c r="E130" t="n">
-        <v>0.5966542750929368</v>
+        <v>0.5584415584415584</v>
       </c>
     </row>
     <row r="131">
@@ -2658,16 +2658,16 @@
         <v>129</v>
       </c>
       <c r="B131" t="n">
-        <v>0.1237439692896955</v>
+        <v>0.1248146310886916</v>
       </c>
       <c r="C131" t="n">
-        <v>0.1281926052437888</v>
+        <v>0.1346750557422638</v>
       </c>
       <c r="D131" t="n">
-        <v>0.57169373549884</v>
+        <v>0.5840297121634169</v>
       </c>
       <c r="E131" t="n">
-        <v>0.5985130111524164</v>
+        <v>0.5584415584415584</v>
       </c>
     </row>
     <row r="132">
@@ -2675,16 +2675,16 @@
         <v>130</v>
       </c>
       <c r="B132" t="n">
-        <v>0.122403732555754</v>
+        <v>0.1261616627521375</v>
       </c>
       <c r="C132" t="n">
-        <v>0.1282754126522276</v>
+        <v>0.1344409154521095</v>
       </c>
       <c r="D132" t="n">
-        <v>0.5819025522041763</v>
+        <v>0.5775301764159703</v>
       </c>
       <c r="E132" t="n">
-        <v>0.5966542750929368</v>
+        <v>0.5584415584415584</v>
       </c>
     </row>
     <row r="133">
@@ -2692,16 +2692,16 @@
         <v>131</v>
       </c>
       <c r="B133" t="n">
-        <v>0.1221310342935955</v>
+        <v>0.1258740955415894</v>
       </c>
       <c r="C133" t="n">
-        <v>0.1273240082793766</v>
+        <v>0.1349817365407944</v>
       </c>
       <c r="D133" t="n">
-        <v>0.5888631090487239</v>
+        <v>0.5951717734447539</v>
       </c>
       <c r="E133" t="n">
-        <v>0.6059479553903345</v>
+        <v>0.5547309833024119</v>
       </c>
     </row>
     <row r="134">
@@ -2709,16 +2709,16 @@
         <v>132</v>
       </c>
       <c r="B134" t="n">
-        <v>0.1217356284751612</v>
+        <v>0.1273632634650259</v>
       </c>
       <c r="C134" t="n">
-        <v>0.1274677978621589</v>
+        <v>0.134388778772619</v>
       </c>
       <c r="D134" t="n">
-        <v>0.5851508120649652</v>
+        <v>0.585422469823584</v>
       </c>
       <c r="E134" t="n">
-        <v>0.5985130111524164</v>
+        <v>0.5547309833024119</v>
       </c>
     </row>
     <row r="135">
@@ -2726,16 +2726,16 @@
         <v>133</v>
       </c>
       <c r="B135" t="n">
-        <v>0.1220062852782362</v>
+        <v>0.1266335726660841</v>
       </c>
       <c r="C135" t="n">
-        <v>0.1276277949412664</v>
+        <v>0.1346906771262487</v>
       </c>
       <c r="D135" t="n">
-        <v>0.5967517401392112</v>
+        <v>0.5784586815227484</v>
       </c>
       <c r="E135" t="n">
-        <v>0.6022304832713755</v>
+        <v>0.5473098330241187</v>
       </c>
     </row>
     <row r="136">
@@ -2743,16 +2743,16 @@
         <v>134</v>
       </c>
       <c r="B136" t="n">
-        <v>0.1215328852481702</v>
+        <v>0.1272351901759119</v>
       </c>
       <c r="C136" t="n">
-        <v>0.1273597967293527</v>
+        <v>0.1343573464287652</v>
       </c>
       <c r="D136" t="n">
-        <v>0.5860788863109049</v>
+        <v>0.5761374187558032</v>
       </c>
       <c r="E136" t="n">
-        <v>0.6003717472118959</v>
+        <v>0.5565862708719852</v>
       </c>
     </row>
     <row r="137">
@@ -2760,16 +2760,16 @@
         <v>135</v>
       </c>
       <c r="B137" t="n">
-        <v>0.120762994622483</v>
+        <v>0.125172502196887</v>
       </c>
       <c r="C137" t="n">
-        <v>0.1279648707972633</v>
+        <v>0.1344346031546593</v>
       </c>
       <c r="D137" t="n">
-        <v>0.5888631090487239</v>
+        <v>0.575208913649025</v>
       </c>
       <c r="E137" t="n">
-        <v>0.5892193308550185</v>
+        <v>0.549165120593692</v>
       </c>
     </row>
     <row r="138">
@@ -2777,16 +2777,16 @@
         <v>136</v>
       </c>
       <c r="B138" t="n">
-        <v>0.1224551148274366</v>
+        <v>0.1260892012540032</v>
       </c>
       <c r="C138" t="n">
-        <v>0.1272429815597004</v>
+        <v>0.1344849301709069</v>
       </c>
       <c r="D138" t="n">
-        <v>0.5837587006960557</v>
+        <v>0.5877437325905293</v>
       </c>
       <c r="E138" t="n">
-        <v>0.6003717472118959</v>
+        <v>0.5528756957328386</v>
       </c>
     </row>
     <row r="139">
@@ -2794,16 +2794,16 @@
         <v>137</v>
       </c>
       <c r="B139" t="n">
-        <v>0.122210510294227</v>
+        <v>0.124224068268257</v>
       </c>
       <c r="C139" t="n">
-        <v>0.1276014985309707</v>
+        <v>0.1346745325459374</v>
       </c>
       <c r="D139" t="n">
-        <v>0.5893271461716937</v>
+        <v>0.5868152274837511</v>
       </c>
       <c r="E139" t="n">
-        <v>0.5985130111524164</v>
+        <v>0.5584415584415584</v>
       </c>
     </row>
     <row r="140">
@@ -2811,16 +2811,16 @@
         <v>138</v>
       </c>
       <c r="B140" t="n">
-        <v>0.1204519138178405</v>
+        <v>0.1257564453955959</v>
       </c>
       <c r="C140" t="n">
-        <v>0.1274766243166394</v>
+        <v>0.1340107892950376</v>
       </c>
       <c r="D140" t="n">
-        <v>0.5925754060324826</v>
+        <v>0.5705663881151346</v>
       </c>
       <c r="E140" t="n">
-        <v>0.5910780669144982</v>
+        <v>0.5640074211502782</v>
       </c>
     </row>
     <row r="141">
@@ -2828,16 +2828,16 @@
         <v>139</v>
       </c>
       <c r="B141" t="n">
-        <v>0.1243442991638885</v>
+        <v>0.1233552367809941</v>
       </c>
       <c r="C141" t="n">
-        <v>0.1269997068577343</v>
+        <v>0.1347290832135412</v>
       </c>
       <c r="D141" t="n">
-        <v>0.5698375870069605</v>
+        <v>0.6044568245125348</v>
       </c>
       <c r="E141" t="n">
-        <v>0.5966542750929368</v>
+        <v>0.5602968460111317</v>
       </c>
     </row>
     <row r="142">
@@ -2845,16 +2845,16 @@
         <v>140</v>
       </c>
       <c r="B142" t="n">
-        <v>0.122272940023857</v>
+        <v>0.1243427601807258</v>
       </c>
       <c r="C142" t="n">
-        <v>0.1278189818064372</v>
+        <v>0.1347957187228733</v>
       </c>
       <c r="D142" t="n">
-        <v>0.5962877030162413</v>
+        <v>0.5988857938718662</v>
       </c>
       <c r="E142" t="n">
-        <v>0.5985130111524164</v>
+        <v>0.5547309833024119</v>
       </c>
     </row>
     <row r="143">
@@ -2862,16 +2862,16 @@
         <v>141</v>
       </c>
       <c r="B143" t="n">
-        <v>0.1203286985264105</v>
+        <v>0.1254468424355283</v>
       </c>
       <c r="C143" t="n">
-        <v>0.1278771857420603</v>
+        <v>0.1343177325195736</v>
       </c>
       <c r="D143" t="n">
-        <v>0.588399071925754</v>
+        <v>0.5909935004642526</v>
       </c>
       <c r="E143" t="n">
-        <v>0.5985130111524164</v>
+        <v>0.5547309833024119</v>
       </c>
     </row>
     <row r="144">
@@ -2879,16 +2879,16 @@
         <v>142</v>
       </c>
       <c r="B144" t="n">
-        <v>0.121195833910914</v>
+        <v>0.1247543418670402</v>
       </c>
       <c r="C144" t="n">
-        <v>0.1276777527398533</v>
+        <v>0.1339956762062179</v>
       </c>
       <c r="D144" t="n">
-        <v>0.582830626450116</v>
+        <v>0.585422469823584</v>
       </c>
       <c r="E144" t="n">
-        <v>0.5985130111524164</v>
+        <v>0.5658627087198516</v>
       </c>
     </row>
     <row r="145">
@@ -2896,16 +2896,16 @@
         <v>143</v>
       </c>
       <c r="B145" t="n">
-        <v>0.1202386733801926</v>
+        <v>0.1259129877914401</v>
       </c>
       <c r="C145" t="n">
-        <v>0.1280561619334751</v>
+        <v>0.1339544049567646</v>
       </c>
       <c r="D145" t="n">
-        <v>0.5851508120649652</v>
+        <v>0.5803156917363046</v>
       </c>
       <c r="E145" t="n">
-        <v>0.5892193308550185</v>
+        <v>0.5602968460111317</v>
       </c>
     </row>
     <row r="146">
@@ -2913,16 +2913,16 @@
         <v>144</v>
       </c>
       <c r="B146" t="n">
-        <v>0.120974247727324</v>
+        <v>0.1230592074639657</v>
       </c>
       <c r="C146" t="n">
-        <v>0.1277157382832633</v>
+        <v>0.1344195960296525</v>
       </c>
       <c r="D146" t="n">
-        <v>0.5832946635730858</v>
+        <v>0.5923862581244197</v>
       </c>
       <c r="E146" t="n">
-        <v>0.5966542750929368</v>
+        <v>0.5602968460111317</v>
       </c>
     </row>
     <row r="147">
@@ -2930,16 +2930,16 @@
         <v>145</v>
       </c>
       <c r="B147" t="n">
-        <v>0.120977250749574</v>
+        <v>0.123323302496882</v>
       </c>
       <c r="C147" t="n">
-        <v>0.1277734670374129</v>
+        <v>0.1339016440841887</v>
       </c>
       <c r="D147" t="n">
-        <v>0.5921113689095128</v>
+        <v>0.6007428040854225</v>
       </c>
       <c r="E147" t="n">
-        <v>0.5947955390334573</v>
+        <v>0.5658627087198516</v>
       </c>
     </row>
     <row r="148">
@@ -2947,16 +2947,16 @@
         <v>146</v>
       </c>
       <c r="B148" t="n">
-        <v>0.1204040087759495</v>
+        <v>0.1228852044133579</v>
       </c>
       <c r="C148" t="n">
-        <v>0.1275035159455405</v>
+        <v>0.134308945801523</v>
       </c>
       <c r="D148" t="n">
-        <v>0.5893271461716937</v>
+        <v>0.6039925719591458</v>
       </c>
       <c r="E148" t="n">
-        <v>0.5985130111524164</v>
+        <v>0.5510204081632653</v>
       </c>
     </row>
     <row r="149">
@@ -2964,16 +2964,16 @@
         <v>147</v>
       </c>
       <c r="B149" t="n">
-        <v>0.1216573566198349</v>
+        <v>0.1259227958233917</v>
       </c>
       <c r="C149" t="n">
-        <v>0.1274964561065038</v>
+        <v>0.1341177167163955</v>
       </c>
       <c r="D149" t="n">
-        <v>0.5819025522041763</v>
+        <v>0.585422469823584</v>
       </c>
       <c r="E149" t="n">
-        <v>0.6003717472118959</v>
+        <v>0.5547309833024119</v>
       </c>
     </row>
     <row r="150">
@@ -2981,16 +2981,16 @@
         <v>148</v>
       </c>
       <c r="B150" t="n">
-        <v>0.121041802360731</v>
+        <v>0.1228721507770174</v>
       </c>
       <c r="C150" t="n">
-        <v>0.127709620528751</v>
+        <v>0.1335339860783683</v>
       </c>
       <c r="D150" t="n">
-        <v>0.5832946635730858</v>
+        <v>0.5942432683379758</v>
       </c>
       <c r="E150" t="n">
-        <v>0.5985130111524164</v>
+        <v>0.5584415584415584</v>
       </c>
     </row>
     <row r="151">
@@ -2998,16 +2998,16 @@
         <v>149</v>
       </c>
       <c r="B151" t="n">
-        <v>0.1201839797637042</v>
+        <v>0.1246181268464116</v>
       </c>
       <c r="C151" t="n">
-        <v>0.1273195801509751</v>
+        <v>0.1336281473437945</v>
       </c>
       <c r="D151" t="n">
-        <v>0.582830626450116</v>
+        <v>0.5923862581244197</v>
       </c>
       <c r="E151" t="n">
-        <v>0.6115241635687733</v>
+        <v>0.5602968460111317</v>
       </c>
     </row>
     <row r="152">
@@ -3015,16 +3015,16 @@
         <v>150</v>
       </c>
       <c r="B152" t="n">
-        <v>0.1197901668355745</v>
+        <v>0.1241030848639853</v>
       </c>
       <c r="C152" t="n">
-        <v>0.127493475874265</v>
+        <v>0.1335246157315042</v>
       </c>
       <c r="D152" t="n">
-        <v>0.5953596287703016</v>
+        <v>0.5868152274837511</v>
       </c>
       <c r="E152" t="n">
-        <v>0.5947955390334573</v>
+        <v>0.5602968460111317</v>
       </c>
     </row>
   </sheetData>

</xml_diff>